<commit_message>
Fixed ITs, Slot IT is making problems yet. ToBe resolved when Slots DataLoader is reworked
</commit_message>
<xml_diff>
--- a/conf-core/src/test/resources/dataloader/conf-data-properties.xlsx
+++ b/conf-core/src/test/resources/dataloader/conf-data-properties.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="3720" yWindow="2625" windowWidth="19020" windowHeight="10110"/>
+    <workbookView xWindow="3720" yWindow="2628" windowWidth="19020" windowHeight="10116"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="97">
   <si>
     <t>HEADER</t>
   </si>
@@ -325,9 +325,6 @@
   </si>
   <si>
     <t>Integer</t>
-  </si>
-  <si>
-    <t>URL</t>
   </si>
   <si>
     <t>Strings List</t>
@@ -700,20 +697,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N27" sqref="N27"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="43.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="43.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B1" s="6" t="s">
         <v>8</v>
       </c>
@@ -721,7 +718,7 @@
       <c r="D1" s="6"/>
       <c r="E1" s="6"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>9</v>
       </c>
@@ -729,7 +726,7 @@
         <v>41304</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -749,7 +746,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>10</v>
       </c>
@@ -766,7 +763,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>2</v>
       </c>
@@ -786,7 +783,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>2</v>
       </c>
@@ -807,7 +804,7 @@
       </c>
       <c r="G9" s="3"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>2</v>
       </c>
@@ -825,7 +822,7 @@
       </c>
       <c r="G10" s="3"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>2</v>
       </c>
@@ -845,7 +842,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>2</v>
       </c>
@@ -865,7 +862,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>2</v>
       </c>
@@ -885,7 +882,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>2</v>
       </c>
@@ -905,7 +902,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>2</v>
       </c>
@@ -922,10 +919,10 @@
         <v>80</v>
       </c>
       <c r="F15" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>2</v>
       </c>
@@ -945,7 +942,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>2</v>
       </c>
@@ -965,7 +962,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>2</v>
       </c>
@@ -985,7 +982,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>2</v>
       </c>
@@ -1005,7 +1002,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>2</v>
       </c>
@@ -1025,7 +1022,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>2</v>
       </c>
@@ -1045,7 +1042,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>2</v>
       </c>
@@ -1065,7 +1062,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>2</v>
       </c>
@@ -1085,7 +1082,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>2</v>
       </c>
@@ -1102,7 +1099,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>2</v>
       </c>
@@ -1122,7 +1119,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>2</v>
       </c>
@@ -1142,7 +1139,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>2</v>
       </c>
@@ -1162,7 +1159,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>2</v>
       </c>
@@ -1182,7 +1179,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>2</v>
       </c>
@@ -1202,7 +1199,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>2</v>
       </c>
@@ -1223,7 +1220,7 @@
       </c>
       <c r="G30" s="1"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>2</v>
       </c>
@@ -1244,7 +1241,7 @@
       </c>
       <c r="G31" s="1"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>2</v>
       </c>
@@ -1265,7 +1262,7 @@
       </c>
       <c r="G32" s="1"/>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>2</v>
       </c>
@@ -1286,7 +1283,7 @@
       </c>
       <c r="G33" s="1"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>2</v>
       </c>
@@ -1307,7 +1304,7 @@
       </c>
       <c r="G34" s="1"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>2</v>
       </c>
@@ -1325,7 +1322,7 @@
       </c>
       <c r="G35" s="1"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>2</v>
       </c>
@@ -1339,11 +1336,11 @@
         <v>90</v>
       </c>
       <c r="F36" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G36" s="1"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>2</v>
       </c>
@@ -1364,7 +1361,7 @@
       </c>
       <c r="G37" s="1"/>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>2</v>
       </c>
@@ -1385,7 +1382,7 @@
       </c>
       <c r="G38" s="1"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>78</v>
       </c>
@@ -1404,7 +1401,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1416,7 +1413,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>